<commit_message>
Added semester-config.py script which can be used to create new semester entries in DB.
</commit_message>
<xml_diff>
--- a/student-config.xlsx
+++ b/student-config.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
+    <sheet name="semester" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
   <si>
     <t>rohsurve</t>
   </si>
@@ -314,6 +315,27 @@
   </si>
   <si>
     <t>Rohit_2</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>SEASON</t>
+  </si>
+  <si>
+    <t>COURSE_NO</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>P532</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>P632</t>
   </si>
 </sst>
 </file>
@@ -685,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,4 +1141,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2016</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2016</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified student-config.py. - Resolved a bug which was losing enrollment table records.
</commit_message>
<xml_diff>
--- a/student-config.xlsx
+++ b/student-config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>rohsurve</t>
   </si>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +743,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
@@ -930,7 +930,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>0</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>5</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>62</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>10</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>2</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
@@ -1145,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B2" t="s">
         <v>103</v>
@@ -1187,17 +1187,6 @@
       </c>
       <c r="C3" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2017</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>